<commit_message>
Border and color fill not working
</commit_message>
<xml_diff>
--- a/in/a.xlsx
+++ b/in/a.xlsx
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -55,13 +55,46 @@
       <b val="1"/>
       <sz val="12"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.3999755851924192"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor rgb="ff330000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <bgColor rgb="00ff3300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="00ffffff"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -88,18 +121,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
+    <xf borderId="0" fillId="6" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle hidden="0" name="highlight" xfId="1"/>
+    <cellStyle builtinId="52" hidden="0" name="60 % - Accent6" xfId="2"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -372,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
@@ -380,7 +424,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:13">
       <c r="A2" t="n">
         <v>12</v>
       </c>
@@ -426,7 +470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" t="n">
         <v>24</v>
       </c>
@@ -449,7 +493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" t="n">
         <v>4344</v>
       </c>
@@ -472,7 +516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" t="n">
         <v>5792</v>
       </c>
@@ -495,7 +539,7 @@
         <v>25.6666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:13">
       <c r="A6" t="n">
         <v>7958</v>
       </c>
@@ -518,7 +562,7 @@
         <v>27.1666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:13">
       <c r="A7" t="n">
         <v>10124</v>
       </c>
@@ -541,7 +585,7 @@
         <v>28.6666666666667</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:13">
       <c r="A8" t="n">
         <v>12290</v>
       </c>
@@ -564,7 +608,7 @@
         <v>30.1666666666667</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:13">
       <c r="A9" t="n">
         <v>14456</v>
       </c>
@@ -587,7 +631,7 @@
         <v>31.6666666666667</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:13">
       <c r="A10" t="n">
         <v>16622</v>
       </c>
@@ -610,7 +654,7 @@
         <v>33.1666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:13">
       <c r="A11" t="n">
         <v>18788</v>
       </c>
@@ -633,7 +677,7 @@
         <v>34.6666666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:13">
       <c r="A12" t="n">
         <v>20954</v>
       </c>
@@ -656,7 +700,7 @@
         <v>36.1666666666667</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:13">
       <c r="A13" t="n">
         <v>23120</v>
       </c>
@@ -679,7 +723,7 @@
         <v>37.6666666666667</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:13">
       <c r="A14" t="n">
         <v>25286</v>
       </c>
@@ -702,7 +746,7 @@
         <v>39.1666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:13">
       <c r="A15" t="n">
         <v>27452</v>
       </c>
@@ -725,7 +769,7 @@
         <v>40.6666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:13">
       <c r="A16" t="n">
         <v>29618</v>
       </c>
@@ -748,7 +792,7 @@
         <v>42.1666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:13">
       <c r="A17" t="n">
         <v>31784</v>
       </c>
@@ -771,7 +815,7 @@
         <v>43.6666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:13">
       <c r="A18" t="n">
         <v>33950</v>
       </c>
@@ -794,7 +838,7 @@
         <v>45.1666666666667</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:13">
       <c r="A19" t="n">
         <v>36116</v>
       </c>
@@ -817,7 +861,7 @@
         <v>46.6666666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:13">
       <c r="A20" t="n">
         <v>38282</v>
       </c>
@@ -840,7 +884,7 @@
         <v>48.1666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:13">
       <c r="A21" t="n">
         <v>40448</v>
       </c>
@@ -863,7 +907,7 @@
         <v>49.6666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:13">
       <c r="A22" t="n">
         <v>42614</v>
       </c>
@@ -886,7 +930,7 @@
         <v>51.1666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:13">
       <c r="A23" t="n">
         <v>44780</v>
       </c>
@@ -909,7 +953,7 @@
         <v>52.6666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:13">
       <c r="A24" t="n">
         <v>46946</v>
       </c>
@@ -932,7 +976,7 @@
         <v>54.1666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:13">
       <c r="A25" t="n">
         <v>49112</v>
       </c>
@@ -955,7 +999,7 @@
         <v>55.6666666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:13">
       <c r="A26" t="n">
         <v>51278</v>
       </c>
@@ -978,7 +1022,7 @@
         <v>57.1666666666667</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:13">
       <c r="A27" t="n">
         <v>53444</v>
       </c>
@@ -1001,30 +1045,45 @@
         <v>58.6666666666667</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:13">
       <c r="A28" t="n">
         <v>55610</v>
       </c>
       <c r="B28" t="n">
         <v>75486.6666666667</v>
       </c>
-      <c r="C28" t="n">
-        <v>66563.55555555561</v>
+      <c r="C28" s="5">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
       </c>
       <c r="D28" t="n">
         <v>76840.29629629639</v>
       </c>
-      <c r="E28" t="n">
-        <v>84877.53086419719</v>
+      <c r="E28" s="5">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
       </c>
       <c r="F28" t="n">
         <v>40.1666666666667</v>
       </c>
-      <c r="G28" t="n">
-        <v>60.1666666666667</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="G28" s="5">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
+      </c>
+      <c r="I28" s="5">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
+      </c>
+      <c r="K28" s="5">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
+      </c>
+      <c r="M28" s="9">
+        <f>COUNTA(C8:C24)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" t="n">
         <v>57776</v>
       </c>
@@ -1047,7 +1106,7 @@
         <v>61.6666666666668</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:13">
       <c r="A30" t="n">
         <v>59942</v>
       </c>

</xml_diff>